<commit_message>
Edited AMFOSTER BUDGET 2024.xlsx
</commit_message>
<xml_diff>
--- a/AMFOSTER BUDGET 2024.xlsx
+++ b/AMFOSTER BUDGET 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\funsa\OneDrive\Desktop\bola\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myRepos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5130DE34-17AB-4290-A233-0473990E7E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0789B658-D0DD-4A3F-8DDE-BBF4D8C4431F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{301F9A93-6F27-43D7-B6A1-C192EF77CCB4}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{301F9A93-6F27-43D7-B6A1-C192EF77CCB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -703,7 +703,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1087,7 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="10">
-        <v>332.05</v>
+        <v>222</v>
       </c>
       <c r="G22" s="15">
         <f>SUM(G13:G21)</f>
@@ -1179,7 +1179,7 @@
       <c r="D28" s="4"/>
       <c r="E28" s="10">
         <f>SUM(E10:E27)</f>
-        <v>5051.12</v>
+        <v>4941.07</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="24" t="s">
@@ -1320,7 +1320,7 @@
       <c r="F39" s="4"/>
       <c r="G39" s="22">
         <f>E7-E28-E36</f>
-        <v>223.03999999999996</v>
+        <v>333.09000000000015</v>
       </c>
     </row>
   </sheetData>
@@ -1336,14 +1336,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="91ebce61-ab24-4817-b4d1-93b60ef5c8f2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001A9A8A9BBE2E3D47800FC740E38E8E2E" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a7d3a4dfd5cfdd0552c6a82ab9dd25b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="91ebce61-ab24-4817-b4d1-93b60ef5c8f2" xmlns:ns4="df12237c-dbe9-4fc3-9025-3914908a08d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ed7f552eb89ae66beab67a481b1eea9" ns3:_="" ns4:_="">
     <xsd:import namespace="91ebce61-ab24-4817-b4d1-93b60ef5c8f2"/>
@@ -1532,6 +1524,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="91ebce61-ab24-4817-b4d1-93b60ef5c8f2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1542,23 +1542,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3184E9EC-1F57-43F3-B581-F27E465814CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="df12237c-dbe9-4fc3-9025-3914908a08d6"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="91ebce61-ab24-4817-b4d1-93b60ef5c8f2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FC3B142-37C9-4428-860A-D023877B4473}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1577,6 +1560,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3184E9EC-1F57-43F3-B581-F27E465814CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="df12237c-dbe9-4fc3-9025-3914908a08d6"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="91ebce61-ab24-4817-b4d1-93b60ef5c8f2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D39AAEF7-02AB-4DE4-9818-99175E71FEDB}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Changed the emergence number
</commit_message>
<xml_diff>
--- a/AMFOSTER BUDGET 2024.xlsx
+++ b/AMFOSTER BUDGET 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myRepos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0789B658-D0DD-4A3F-8DDE-BBF4D8C4431F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E157841C-4C96-41B6-B068-B7408BFE7338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{301F9A93-6F27-43D7-B6A1-C192EF77CCB4}"/>
   </bookViews>
@@ -702,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A7743AE-D3CA-407C-9837-1781B4A18FF1}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,7 +1250,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="10">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -1277,7 +1277,7 @@
       <c r="A36" s="3"/>
       <c r="B36" s="18">
         <f>SUM(B33:B35)</f>
-        <v>1183</v>
+        <v>1383</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -1312,7 +1312,7 @@
       </c>
       <c r="B39" s="7">
         <f>B7-B28-B36</f>
-        <v>25.639999999999418</v>
+        <v>-174.36000000000058</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="20"/>
@@ -1336,6 +1336,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="91ebce61-ab24-4817-b4d1-93b60ef5c8f2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001A9A8A9BBE2E3D47800FC740E38E8E2E" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a7d3a4dfd5cfdd0552c6a82ab9dd25b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="91ebce61-ab24-4817-b4d1-93b60ef5c8f2" xmlns:ns4="df12237c-dbe9-4fc3-9025-3914908a08d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ed7f552eb89ae66beab67a481b1eea9" ns3:_="" ns4:_="">
     <xsd:import namespace="91ebce61-ab24-4817-b4d1-93b60ef5c8f2"/>
@@ -1524,38 +1541,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="91ebce61-ab24-4817-b4d1-93b60ef5c8f2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FC3B142-37C9-4428-860A-D023877B4473}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D39AAEF7-02AB-4DE4-9818-99175E71FEDB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="91ebce61-ab24-4817-b4d1-93b60ef5c8f2"/>
-    <ds:schemaRef ds:uri="df12237c-dbe9-4fc3-9025-3914908a08d6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1578,9 +1567,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D39AAEF7-02AB-4DE4-9818-99175E71FEDB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FC3B142-37C9-4428-860A-D023877B4473}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="91ebce61-ab24-4817-b4d1-93b60ef5c8f2"/>
+    <ds:schemaRef ds:uri="df12237c-dbe9-4fc3-9025-3914908a08d6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>